<commit_message>
Kalfat! Wszystko poprawiłem prócz scenariusza 11 >.< Trzeba tam wcisnąć dialogi od Wydry przez poprawą tych polskich rzeczy. Błagam Cię, ogarnij to.
</commit_message>
<xml_diff>
--- a/storyboard and dialogues/Tłumaczenia Wydry/Reszta polskich poprawek.xlsx
+++ b/storyboard and dialogues/Tłumaczenia Wydry/Reszta polskich poprawek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408F1D72-4AC7-470C-AA28-6C3AF50AE160}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D29D16-27E7-4041-AA6A-25D1E15CC8AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="10185" tabRatio="500" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="10185" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="07" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="1473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1474">
   <si>
     <t>Event/Description</t>
   </si>
@@ -6338,93 +6338,21 @@
     <t>Epilogue</t>
   </si>
   <si>
-    <t>Świat nigdy nie poznał prawdy o dniu, w którym nadzieje Wielkiej Hordy zostały obrócone w pył. Powszechnie mówiło się o zdradzie Gewolda oraz pułapce, jaką przygotował dla Wielkiego Suwerena. Z masakry miał nie ostać się żaden wojownik, zaś władcy północy jednogłośnie uznali, iż Marbus zginął chwalebną śmiercią, za którą należy mu się cześć i chwała. Został on uznany za wielkiego bohatera, a jego wizerunek posłużył do tego, by stopniowo narzucać pęta na rasę orków i przejmować coraz to większą nad nią kontrolę.</t>
-  </si>
-  <si>
-    <t>Po śmierci Marbusa i Gewolda Wielka Horda przeżyła rozłam. Pomniejsze klany orków nie potrafiły się już zjednoczyć. Nie znalazł się nikt na tyle charyzmatyczny, by tego dokonać. Wkrótce Sojusz Północy objął pieczę nad większą częścią tej rasy, starając się utrzymać ją w ryzach i nigdy więcej nie dopuścić do tego, by Wielka Horda zebrała się ponownie. Wszyscy, którzy stawiali opór owym zmianom, zostali uznani za wrogów ideologi Marbusa i byli szybko eliminowani.</t>
-  </si>
-  <si>
-    <t>Córki Aidali znały jednak prawdę. Przysięgły zemstę na Elfich Jarlach i przez kolejne lata skutecznie walczyły z nimi na morzu i w innych zbiornikach wodnych. Zemsta jednak nie opłaciła im się- szybko zostały uznane za zdrajczynie i wrogów północy. Bez sojusznika w postaci orków, nagi stały się łatwym celem dla łowców głów i najemników. Ich rasa zaczęła karleć, by w końcu odejść w zapomnienie.</t>
-  </si>
-  <si>
-    <t>Jaszczury mocno zintegrowały się z klanami orków. Ich los splótł się z nimi i doprowadził pod jarzmo Sojuszu Północy, gdzie dotknął ich rasizm i seria prześladowań, głównie ze strony magów i uczonych, którzy wyśmiewali prymitywną magię oraz wierzenia jaszczurzych szamanów. Choć ich rasa mogła teraz wędrować po całej północy bez przeszkód, żaden jej przedstawiciel nie czuł się naprawdę wolny.</t>
-  </si>
-  <si>
-    <t>Rasa trolli niemal całkowicie odeszła w zapomnienie. Nie przyłączając się do Wielkiej Hordy, trolle ciągle były uważane za dzikie, wrogo nastawione stworzenia, które trzeba wytępić. Ich plemiona coraz skuteczniej były spychane pod ziemię bądź na najodleglejszą północ, gdzie klimat wybijał je równie skutecznie, co krasnoludzkie młoty. W niedługim czasie rasa odeszła w zapomnienie i tylko stare niańki opowiadały przy ogniskach niestworzone historie o olbrzymach z kamienia.</t>
-  </si>
-  <si>
-    <t>Jaszczury nie zintegrowały się z klanami orków, przez co nie zostały wcielone w szeregi Wielkiej Hordy. Przez możnowładców północy zostały uznane za potencjalne zagrożenie, z którym należało się czym prędzej rozprawić. W skutek działań Sojuszu Północy zginęło znacznie więcej przedstawicieli tej rasy, niźli od miecza wojowników Dzikiego Gonu. Ostatnie klany jaszczurów emigrowały na południe, a także na bardzo daleki wschód - w stronę skażonych, ciągnących się kilometrami moczar, gdzie czekała ich niepewna przyszłość.</t>
-  </si>
-  <si>
-    <t>Trolle zjednoczyły się z Wielką Hordą i bez sprzeciwu przyjmowały rozkazy od swoich nowych panów. Tymi zaś byli najczęściej wysokiej rangi magami Sojuszu Północy, którzy zapewnili im wikt i opierunek, choć żądali za to wysokiej ceny... Stworzony i włączony w życie został program edukacyjny, którego celem miało być ograniczenie intelektu tej rasy i przystosowanie ich do życia w społeczeństwie przyszłości, a zatem takim, w którym trolle stałyby się sługami ludzi, elfów i krasnoludów. Choć w końcu miały mnóstwo żywności, trzymano ich na krótkim łańcuchu, który z czasem miał zamienić się w kajdany.</t>
-  </si>
-  <si>
-    <t>Zły los nie minął Krwawych Elfów. Pozbawieni przywódczyni, szybko nastawili się przeciwko sobie i wzajemnie wybili. Ci, którzy przetrwali, zostali nazwani bandytami oraz zdrajcami elfiej rasy. Czerwony Kapturek, ostatnia potomkini Landara, stała się symbolem zdrady, młodzieńczej głupoty i nienawiści. Wkrótce wszyscy zapomnieli o szacunku, jaki budziła, a dzieci zaczęły bawić się w "Czerwonego Kapturka i wilka". W owej zabawie nie chodziło jednak ani o rewolucję i walkę przeciwko Elfickim Jarlom, ani o ideały Landara.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krwawe Elfy pod przewodnictwem Czerwonego Kapturka stały się jedną z największych sił militarnych północy. Przynajmniej do czasu, aż rozprawili się już ze wszystkimi potencjalnymi zagrożeniami. Po kilku latach walk na każdym możliwym froncie, potomkini Landara zaczęła walczyć o należne sobie prawa. Jak łatwo można się było domyślić - bezskutecznie. Szybko zyskała sobie przydomek "buntowniczki bez powodu" i po kilku próbach wzniecenia buntu wśród elfów, została w końcu skazana na wygnanie. </t>
-  </si>
-  <si>
-    <t>Sojusz Północy, Elficcy Jarlowie oraz Knalga przeżywały rozkwit. Dziki Gon zadał im olbrzymie straty, jednak znacznie bardziej dotknął wszystkich tych, z którymi owe państwa toczyły wojny. Wkrótce nawiązano nowe sojusze, układy i organizacje, które miały umocnić więź powstałą pomiędzy wszystkimi krainami północy. Pod przewodnictwem Jarlów, Królów i Lordów cała północ pławiła się w dostatku. Przynajmniej do czasu, gdy nie pojawi się nowe zagrożenie bądź konflikt zbrojny…</t>
-  </si>
-  <si>
-    <t>Róg Gjallarhorn został ukryty przez Elfich Jarlów i Najwyższą Kapłankę, Beatrycze. Choć miał przynależeć do rasy orków, żaden z nich miał go nie zobaczyć przez następne tysiąc lat. Dopiero wówczas miano pozwolić na to, by wybrać wśród orków Wielkiego Suwerena. Oczywiście tym razem byłaby to osoba odpowiednio wyselekcjonowana przez władców północy, by nie ważyła się im sprzeciwić oraz nakłonić swoją rasę do buntu.</t>
-  </si>
-  <si>
-    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje wraz ze swym wilkiem przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy Pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne teorie na temat tego tajemniczego jegomościa... Jedni twierdzili, że to właśnie Król Gonu przechadza się po świecie, by zebrać dusze umarłych i wskrzesić ich za następne tysiąc lat... Drudzy sądzili, iż to właśnie Marbus nawiedza północ, by odpokutować za dawne grzechy swojej rasy... O tym jednak nie traktuje już ta opowieść…</t>
-  </si>
-  <si>
-    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje samotnie przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy Pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne teorie na temat tego tajemniczego jegomościa... Jedni twierdzili, że to właśnie Król Gonu przechadza się po świecie, by zebrać dusze umarłych i wskrzesić ich za następne tysiąc lat... Drudzy sądzili, iż to właśnie Marbus nawiedza północ, by odpokutować za dawne grzechy swojej rasy... O tym jednak nie traktuje już ta opowieść…</t>
-  </si>
-  <si>
-    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje wraz ze swym wilkiem przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy Pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne domysły na jego temat, jednak w końcu znalazł się ktoś, kto podjął się zadania wytropienia go i poznania prawdy. Czerwony Kapturek ruszyła jego śladem kilka lat po swoim wygnaniu. Od tego momentu zaczęto rozmawiać o bitwach, które toczyła między sobą ta dwójka, o zmaganiach Potomkini Landara i Tajemniczego Orka. I choć wiele lat minęło, odkąd Czerwony Kapturek poprzysięgła zabicie Marbusa, pogłoski o walkach tej dwójki trwają do dziś.</t>
-  </si>
-  <si>
-    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje samotnie przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy Pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne domysły na jego temat, jednak w końcu znalazł się ktoś, kto podjął się zadania wytropienia go i poznania prawdy. Czerwony Kapturek ruszyła jego śladem kilka lat po swoim wygnaniu. Od tego momentu zaczęto rozmawiać o bitwach, które toczyła między sobą ta dwójka, o zmaganiach Potomkini Landara i Tajemniczego Orka. I choć wiele lat minęło, odkąd Czerwony Kapturek poprzysięgła zabicie Marbusa, pogłoski o walkach tej dwójki trwają do dziś.</t>
-  </si>
-  <si>
-    <t>Pod przewodnictwem Marbusa Wielka Horda szybko stała się największą potęgą północy, z którą liczyć się musiał cały Wielki Kontynent. Takie państwa jak Wesnoth bądź Elensefar próbowały wspomóc rozbity już Sojusz Północy bądź Elfickich Jarlów, jednak na próżno. Wielki Suweren rządził żelazną ręką i jakiekolwiek oznaki buntu były szybko i skutecznie tłamszone. Nie było szans na pokonanie oprawcy, przynajmniej za życia Marbusa.</t>
-  </si>
-  <si>
-    <t>Gewold został dowódcą armii Wielkiego Suwerena. Pod jego rozkazami rasa orków wydała na świat najznamienitszych wojowników i żołnierzy. W historii swojej rasy zapisał się nie tylko jako znakomity przywódca, ale także odnowiciel: zniewolił elfy, krasnoludy i ludzi, a następnie nakazał im tworzyć nowe, potężne fortece, które swoim kształtem i rozmiarem przypominały, a także upamiętniały spalone wcześniej Gelu'Aben.</t>
-  </si>
-  <si>
-    <t>Aidala do końca życia towarzyszyła Wielkiemu Suwerenowi wszędzie tam, gdzie się udał. Nieoficjalnie mówiło się o ich związku, jednak nikt nie zdobyłby się na to, by ich za to piętnować. Wkrótce nagi zalały całą północ, a posągi Aidali, matki nag, wypełniły podwodne zbiorniki i stawiane były u ujścia rzek. Choć jej córki wreszcie były wolne, żadna nie wyrzekła się swojej matki. Wręcz przeciwnie- zdawać by się mogło, że oddają jej wręcz nabożną cześć.</t>
-  </si>
-  <si>
     <t>Emborgi-tarash brała udział w najważniejszych bitwach Wielkiej Hordy oraz wielu tych, o których się nie mówiło. Choć przewidziała swoją śmierć na polu walki, nie znalazła jej. Przynajmniej nie za panowania Marbusa. Pod jej przewodnictwem jaszczury odnowiły swoje sabaty i wierzenia, a także zaludniły północ. Na zawsze stały się częścią Wielkiej Hordy i biada było temu, kto ośmielił się je dyskryminować. W niedługim czasie rasa ta odzyskała swoją potęgę i stała się równie silna, co orkowie.</t>
   </si>
   <si>
     <t>Emborgi-tarash odnalazła swoją śmierć na polu bitwy, tak jak przepowiedziała wiele wieków temu. Jej rasa wznosiła modły, odprawiała rytuały i śpiewy, a w końcu podniosła się z żałoby. Pod przewodnictwem Marbusa jaszczury odzyskały dawną chwałę, odnowiły swoje sabaty i wierzenia, a także zaludniły północ. Na zawsze stały się częścią Wielkiej Hordy i biada było temu, kto ośmielił się je dyskryminować. W niedługim czasie rasa ta odzyskała swoją potęgę i stała się równie silna, co orkowie.</t>
   </si>
   <si>
-    <t>Gdy Wielka Horda podbiła już znaczną część północy, orkowie coraz częściej napotykali na swojej drodze trolli. Pierwsze próby nawiązania z nimi dobrych stosunków spełzły na niczym, jednak Marbus nie poddawał się i ostatecznie doprowadził do tego, że trolle stały się częścią Wielkiej Hordy, współpracowały z orkami i jaszczurami, a także zaludniły sporą część dawnej Knalgi.</t>
-  </si>
-  <si>
-    <t>Krull Skała stanął na czele trolli i stał się pierwszym przedstawicielem tej rasy, który zabłysnął jako emisariusz i dyplomata. Rozmawiał jednak głównie z innymi trollami, które zostały wygnane tak daleko na północ, że niemalże nie wiedziały o Dzikim Gonie i zmianach, jakie nastały po wojnie. Wkrótce Krull Skała zyskał sobie miano Króla Trolli i osiadł ze swoją rasą w dawnej Knaldze, choć wciąż był suwerenem Marbusa. Dwójka ta darzyła się wzajemną przyjaźnią i szacunkiem, aż po kres ich dni.</t>
-  </si>
-  <si>
     <t>Krull Skała zginął u boku Marbusa podczas wojny. Zostawił po sobie jednak liczne potomstwo, a także ideologię, która jasno mówiła, iż trolle powinny zjednoczyć się z Wielką Hordą. Tak właśnie się stało. Wielki Suweren rozkazał wysłać emisariuszy do najdalszych krańców północy i odszukać wszystkie odesłane na wygnanie klany trolli, by sprowadzić je do siebie i zjednoczyć. Choć proces ten trwał latami, w końcu trolle osiadły w dawnej Knaldze i zaludniły ją, wiernie służąc przy tym Marbusowi.</t>
   </si>
   <si>
     <t>Jaszczury, choć nie przynależały do Wielkiej Hordy, gdy Marbus toczył swoje wojny, stały się jej częścią w trakcie pokoju. Powrócono do przyjaźni, która łączyła ich rasę z orkami. W niedługim czasie wierzenia jaszczurów stały się główną religią Wielkiej Hordy, zaś sabaty ich szamanów odbywały się co miesiąc. Wspólnie osiągnęli znacznie więcej, niż udałoby im się zdobyć osobno.</t>
   </si>
   <si>
-    <t>Czerwony Kapturek przeszła do historii jako potomkini Landara, pani Krwawych Elfów i opływająca w bogactwa wojowniczka. Marbus dotrzymał słowa i wysypał przed jej stopami praktycznie całe złoto elfów. Wystarczyłoby go do opłacenia wojska z południa i wzniecenia buntu przeciwko Wielkiej Hordzie, jednak tak się nie stało. Zamiast tego Czerwony Kapturek obwieściła się królową elfów północy, podległą jedynie władzy Wielkiego Suwerena. W niedługim czasie okazało się, że jest jeszcze okrutniejsza niż orkowie. Stała się katem dla własnej rasy.</t>
-  </si>
-  <si>
-    <t>Bez swojej liderki, Krwawe Elfy rozpierzchły się i niemal całkowicie o nich zapomniano. Imię Czerwonego Kapturka nie przeszło do historii, nie zapisała się nawet jedna wzmianka o potomkini Landara oraz jej ideałach. Po latach nikt nie wspominał już ani jej, ani Elfich Jarlów. Rasa elfów stała się jednolitą, szarą masą niewolników, którzy przestali nawet marzyć o odmianie swego losu.</t>
-  </si>
-  <si>
-    <t>Jęczmień do końca swych dni został u boku Marbusa. Przypominał mu o Kochanie i był podporą w trudnych chwilach. Stał się ojcem dla kilkudziesięciu wilcząt, z których każde stało się w przyszłości wierzchowcem dla najlepszych goblińskich jeźdźców.</t>
-  </si>
-  <si>
     <t>Róg Gjallarhorn został ukryty w jednej z twierdz, które zbudował Gewold. Strzegła go potężna magia orków, trolli i jaszczurów. Choć zabezpieczono go najlepiej, jak można było, a wiadomości o nim zapisano w tysiącach ksiąg i zwojów, Marbus nadal obawiał się dnia, w którym Król Gonu pojawi się znowu.</t>
   </si>
   <si>
-    <t>Co zaś tyczy się samego Marbusa... Do końca swojego długiego życia piastował on miejsce Wielkiego Suwerena. Nie miał potomstwa, nie zostawił więc nikogo na miejsce swojego następcy. Władcy klanów orków zebrali się, by spierać się o stanowisko wodza, jednak ostatecznie miejsce to zajęła Aidala. Jako naga, istota długowieczna i kochanka Marbusa, przejęła po nim władze, tłumiąc szybko wszelki opór. Wszystko to należy już jednak do całkiem innej historii…</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
@@ -6434,19 +6362,10 @@
     <t>1b</t>
   </si>
   <si>
-    <t>Gdy Wielka Horda zapanowała na północy, z najdzikszych jej terenów wynurzyły się ogry i inne, rzadziej spotykane stworzenia. Podjęły one samobójczą, z góry przegraną walkę z nowym uzurpatorem. Z roku na rok organizowane były polowania na Yeti’ch, a sala tronowa Marbusa szybko pokryła się trofeami z ich głów. Kolejna rasa upadła pod ciężkimi butami orków.</t>
-  </si>
-  <si>
     <t>1c</t>
   </si>
   <si>
-    <t>Gdy Wielka Horda została rozbita, a potęga orków ponownie przeszła do historii, ogry i Yeti wynurzyły się ze swoich pieczar, by walczyć przeciwko elfickim jarlom. Choć zadawały im duże szkody i zabiły wielu wodzów, ich porażka była nieunikniona. Wkrótce łby potworów stały się trofeami na ścianach wielmożów północy, którzy traktowali ich wyłącznie jako zwierzynę łowną.</t>
-  </si>
-  <si>
     <t>1d</t>
-  </si>
-  <si>
-    <t>Gdy Wielka Horda została rozbita, a potęga orków ponownie przeszła do historii, ogry, Yeti i inne, dzikie rasy północy umknęły w niedostępne dla elfów tereny, gdzie potajemnie mnożyły się bądź wymierały. Wkrótce przeszły do historii, a w kolejnych latach — do legend i bajek dla dzieci. Jarlowie wyparli pamięć o nich, by jeszcze bardziej przyporządkować sobie północne kraje.</t>
   </si>
   <si>
     <t>Nieumarły Dowódca</t>
@@ -7150,6 +7069,90 @@
   </si>
   <si>
     <t>Stałość</t>
+  </si>
+  <si>
+    <t>Alternatywne tytuły:</t>
+  </si>
+  <si>
+    <t>Świat nigdy nie poznał prawdy o dniu, w którym nadzieje Wielkiej Hordy zostały obrócone w pył. Powszechnie mówiło się o zdradzie Gewolda oraz pułapce, jaką przygotował dla Wielkiego Suwerena. Z masakry miał nie ostać się żaden wojownik, zaś władcy północy jednogłośnie uznali, iż Marbus zginął chwalebną śmiercią, za którą należy mu się cześć i chwała. Został on uznany za wielkiego bohatera, a jego wizerunek posłużył do tego, by stopniowo narzucać pęta na rasę orków i przejmować coraz to większą nad nimi kontrolę.</t>
+  </si>
+  <si>
+    <t>Po śmierci Marbusa i Gewolda Wielka Horda przeżyła rozłam. Pomniejsze klany orków nie potrafiły się już zjednoczyć. Nie znalazł się nikt na tyle charyzmatyczny, by tego dokonać. Wkrótce Sojusz Północy objął pieczę nad większą częścią tej rasy, starając się utrzymać ją w ryzach i nigdy więcej nie dopuścić do tego, by orkowie zebrali się ponownie. Wszyscy, którzy stawiali opór owym zmianom, zostali uznani za wrogów ideologii Marbusa i zostawali szybko wyeliminowani.</t>
+  </si>
+  <si>
+    <t>Córki Aidali znały jednak prawdę. Przysięgły zemstę na Elfich Jarlach i przez kolejne lata skutecznie walczyły z nimi na morzu i w innych zbiornikach wodnych. Zemsta jednak nie opłaciła im się – szybko uznano je za zdrajczynie i wrogów północy. Bez sojuszników w postaci orków, nagi stały się łatwym celem dla łowców głów i najemników. Ich rasa zaczęła karleć, by w końcu odejść w zapomnienie.</t>
+  </si>
+  <si>
+    <t>Jaszczury mocno zintegrowały się z klanami orków. Ich los splótł się z nimi i doprowadził pod jarzmo Sojuszu Północy, gdzie dotknął ich rasizm i seria prześladowań, głównie ze strony magów oraz uczonych, którzy wyśmiewali prymitywną magię a także wierzenia jaszczurzych szamanów. Choć ich rasa mogła teraz wędrować po całej północy bez przeszkód, żaden jej przedstawiciel nie czuł się naprawdę wolny.</t>
+  </si>
+  <si>
+    <t>Rasa trolli niemal całkowicie odeszła w zapomnienie. Nie przyłączając się do Wielkiej Hordy, trolle ciągle były uważane za dzikie, wrogo nastawione stworzenia, które trzeba wytępić. Ich plemiona coraz skuteczniej spychano pod ziemię bądź na najodleglejszą północ, gdzie klimat wybijał je równie skutecznie, co krasnoludzkie młoty. W niedługim czasie odeszły w zapomnienie i tylko stare niańki opowiadały przy ogniskach niestworzone historie o olbrzymach z kamienia.</t>
+  </si>
+  <si>
+    <t>Jaszczury nie zintegrowały się z klanami orków, przez co nie zostały wcielone w szeregi Wielkiej Hordy. Przez możnowładców północy zostały uznane za potencjalne zagrożenie, z którym należało się czym prędzej rozprawić. W skutek działań Sojuszu Północy zginęło znacznie więcej przedstawicieli tejże rasy, niźli od mieczy wojowników Dzikiego Gonu. Ostatnie klany jaszczurów emigrowały na południe a także na bardzo daleki wschód – w stronę skażonych, ciągnących się kilometrami moczar, gdzie czekała ich niepewna przyszłość.</t>
+  </si>
+  <si>
+    <t>Trolle zjednoczyły się z Wielką Hordą i bez sprzeciwu przyjmowały rozkazy od swoich nowych panów. Tymi zaś byli najczęściej wysokiej rangi magowie Sojuszu Północy, którzy zapewnili im wikt i opierunek, choć żądali za to wysokiej ceny... Włączony w życie został program edukacyjny, którego celem miało być ograniczenie intelektu tej rasy i przystosowanie ich do życia w społeczeństwie przyszłości, a zatem takim, w którym trolle stałyby się sługami ludzi, elfów i krasnoludów. Choć w końcu miały mnóstwo żywności, trzymano ich na krótkim łańcuchu, który z czasem miał zamienić się w kajdany.</t>
+  </si>
+  <si>
+    <t>Zły los nie minął Krwawych Elfów. Pozbawieni przywódczyni, szybko nastawili się przeciwko sobie i wzajemnie wybili. Ci, którzy przetrwali, zostali nazwani bandytami oraz zdrajcami elfiej rasy. Czerwony Kapturek, ostatnia potomkini Landara, stała się symbolem zdrady, młodzieńczej głupoty i nienawiści. Wkrótce wszyscy zapomnieli o szacunku, jaki budziła, a dzieci zaczęły bawić się w „Czerwonego Kapturka i wilka”. W owej zabawie nie chodziło jednak ani o rewolucję i walkę przeciwko Elfickim Jarlom, ani o ideały Landara.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krwawe Elfy pod przewodnictwem Czerwonego Kapturka stały się jedną z największych sił militarnych północy. Przynajmniej do czasu, gdy rozprawili się ze wszystkimi potencjalnymi zagrożeniami. Po kilku latach walk na każdym możliwym froncie, potomkini Landara zaczęła upominać się o należne sobie prawa. Jak łatwo można się było domyślić – bezskutecznie. Szybko zyskała sobie przydomek „buntowniczki bez powodu” i po kilku próbach wzniecenia rewolucji wśród elfów, została skazana na wygnanie. </t>
+  </si>
+  <si>
+    <t>Sojusz Północy, Elficcy Jarlowie oraz Knalga przeżywały rozkwit. Dziki Gon zadał im olbrzymie straty, jednak znacznie bardziej dotknął wszystkich tych, z którymi owe państwa toczyły wojny. Wkrótce nawiązano nowe sojusze i układy, które miały umocnić więź powstałą pomiędzy wszystkimi krainami północy. Pod przewodnictwem Jarlów, Królów i Lordów wszystkim żyło się lepiej. Przynajmniej do czasu, gdy nie rozpoczęła się kolejna wojna...</t>
+  </si>
+  <si>
+    <t>Róg Gjallarhorn został ukryty przez Elfich Jarlów i Najwyższą Kapłankę, Beatrycze. Choć miał przynależeć do rasy orków, żaden z nich nie miał go zobaczyć przez następne tysiąc lat. Dopiero wówczas miano pozwolić na to, by wybrać wśród orków Wielkiego Suwerena. Oczywiście tym razem byłaby to osoba odpowiednio wyselekcjonowana przez władców północy, by nie ważyła się im sprzeciwić oraz nakłonić swoją rasę do buntu.</t>
+  </si>
+  <si>
+    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje wraz ze swym wilkiem przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne teorie na temat tego tajemniczego jegomościa... Jedni twierdzili, że to właśnie Król Gonu przechadza się po świecie, by zebrać dusze umarłych i wskrzesić ich za następne tysiąc lat... Drudzy sądzili, iż to Marbus nawiedza północ, by odpokutować za dawne grzechy swojej rasy... O tym jednak nie traktuje już ta opowieść…</t>
+  </si>
+  <si>
+    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje samotnie przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne teorie na temat tego tajemniczego jegomościa... Jedni twierdzili, że to właśnie Król Gonu przechadza się po świecie, by zebrać dusze umarłych i wskrzesić ich za następne tysiąc lat... Drudzy sądzili, iż to Marbus nawiedza północ, by odpokutować za dawne grzechy swojej rasy... O tym jednak nie traktuje już ta opowieść…</t>
+  </si>
+  <si>
+    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje wraz ze swym wilkiem przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne domysły na jego temat, jednak w końcu znalazł się ktoś, kto podjął się zadania wytropienia go i poznania prawdy. Czerwony Kapturek ruszyła jego śladem kilka lat po swoim wygnaniu. Od tego momentu zaczęto rozmawiać o bitwach, które toczyła między sobą ta dwójka, o zmaganiach Potomkini Landara i Tajemniczego Orka. I choć wiele lat minęło, odkąd Czerwony Kapturek poprzysięgła zabicie Marbusa, pogłoski o walkach tej dwójki trwają do dziś.</t>
+  </si>
+  <si>
+    <t>Co zaś tyczy się Marbusa... Na północy rozeszła się wieść o tajemniczym orku, który wędruje samotnie przez wszystkie krainy i nosi na piersi magiczny, potężny amulet. Świadkowie opowiadali, że otaczała go lodowata, nieprzenikniona aura, a weterani bitwy pod Górą Przeznaczenia porównywali ją do uczucia, które towarzyszyło im, gdy stanął przed nimi Król Gonu. Snuto różne domysły na jego temat, jednak w końcu znalazł się ktoś, kto podjął się zadania wytropienia go i poznania prawdy. Czerwony Kapturek ruszyła jego śladem kilka lat po swoim wygnaniu. Od tego momentu zaczęto rozmawiać o bitwach, które toczyła między sobą ta dwójka, o zmaganiach Potomkini Landara i Tajemniczego Orka. I choć wiele lat minęło, odkąd Czerwony Kapturek poprzysięgła zabicie Marbusa, pogłoski o walkach tej dwójki trwają do dziś.</t>
+  </si>
+  <si>
+    <t>Pod przewodnictwem Marbusa Wielka Horda szybko stała się największą potęgą północy, z którą liczyć się musiał cały Wielki Kontynent. Takie państwa, jak Wesnoth bądź Elensefar próbowały wspomóc rozbity już Sojusz Północy i Elfickich Jarlów, jednak na próżno. Wielki Suweren rządził żelazną ręką, a jakiekolwiek oznaki buntu były szybko i skutecznie tłamszone. Nie było szans na pokonanie oprawcy, przynajmniej za życia Marbusa.</t>
+  </si>
+  <si>
+    <t>Gewold został dowódcą armii Wielkiego Suwerena. Pod jego rozkazami rasa orków wydała na świat najznamienitszych wojowników i żołnierzy. W historii swojej rasy zapisał się nie tylko jako znakomity przywódca, ale także odnowiciel – zniewolił elfy, krasnoludy i ludzi, a następnie nakazał im tworzyć nowe, potężne fortece, które swoim kształtem i rozmiarem przypominały, a także upamiętniały, spalone wcześniej Gelu'Aben.</t>
+  </si>
+  <si>
+    <t>Aidala do końca życia towarzyszyła Wielkiemu Suwerenowi wszędzie tam, gdzie się udawał. Nieoficjalnie mówiło się o ich związku, jednak nikt nie zdobyłby się na to, by ich za to piętnować. Wkrótce nagi zalały całą północ, a posągi Aidali, Matrony Nag, wypełniły podwodne zbiorniki i stawiane były u ujść rzek. Choć jej córki wreszcie były wolne, żadna z nich nie wyrzekła się swojej matki. Wręcz przeciwnie –  zdawać by się mogło, że oddają jej wręcz nabożną cześć.</t>
+  </si>
+  <si>
+    <t>Gdy Wielka Horda podbiła już znaczną część północy, orkowie coraz częściej napotykali na swojej drodze trolle. Pierwsze próby nawiązania z nimi dobrych stosunków spełzły na niczym, jednak Marbus nie poddawał się i ostatecznie doprowadził do tego, że stały się one częścią Wielkiej Hordy, współpracowały z orkami i jaszczurami, a także zaludniły sporą część dawnej Knalgi.</t>
+  </si>
+  <si>
+    <t>Krull Skała stanął na czele trolli i stał się pierwszym przedstawicielem tej rasy, który zabłysnął jako emisariusz i dyplomata. Rozmawiał jednak głównie z innymi trollami, które zostały wygnane tak daleko na północ, że niemalże nie wiedziały o Dzikim Gonie i zmianach, jakie nastały po wojnie. Wkrótce Krull Skała zyskał sobie miano Króla Trolli i osiadł ze swoją rasą w dawnej Knaldze, choć wciąż był suwerenem Marbusa. Dwójka ta darzyła się wzajemną przyjaźnią i szacunkiem aż po kres ich dni.</t>
+  </si>
+  <si>
+    <t>Czerwony Kapturek przeszła do historii jako potomkini Landara, pani Krwawych Elfów i opływająca w bogactwa wojowniczka. Marbus dotrzymał słowa i wysypał przed jej stopami całe złoto elfów. Wystarczyłoby go do opłacenia wojska z południa i wzniecenia buntu przeciwko Wielkiej Hordzie, jednak tak się nie stało. Zamiast tego Czerwony Kapturek obwieściła się Królową Elfów Północy, podległą jedynie władzy Wielkiego Suwerena. W niedługim czasie okazało się, że jest jeszcze okrutniejsza niż orkowie. Stała się katem dla własnej rasy.</t>
+  </si>
+  <si>
+    <t>Bez swojej liderki Krwawe Elfy rozpierzchły się i niemal całkowicie o nich zapomniano. Imię Czerwonego Kapturka nie przeszło do historii, nie zapisała się nawet jedna wzmianka o potomkini Landara oraz jej ideałach. Po latach nikt nie wspominał już ani jej, ani Elfich Jarlów. Rasa elfów stała się jednolitą, szarą masą niewolników, którzy przestali marzyć o odmianie swego losu.</t>
+  </si>
+  <si>
+    <t>Jęczmień do końca swych dni został u boku Marbusa. Przypominał mu Kochana i był podporą w trudnych chwilach. Stał się ojcem dla kilkudziesięciu wilcząt, z których każde stało się w przyszłości wierzchowcem dla najlepszych goblińskich jeźdźców.</t>
+  </si>
+  <si>
+    <t>Co zaś tyczy się samego Marbusa... Do końca swojego długiego życia piastował on tytuł Wielkiego Suwerena. Nie miał potomstwa, nie zostawił więc nikogo na swoje miejsce. Władcy klanów orków zebrali się, by rozmawiać o stanowisku wodza, jednak ostatecznie miejsce to zajęła Aidala. Jako naga, istota długowieczna i kochanka Marbusa, przejęła po nim władze, tłumiąc szybko wszelki opór. Wszystko to należy już jednak do całkiem innej historii…</t>
+  </si>
+  <si>
+    <t>Gdy Wielka Horda zapanowała na północy, z najdzikszych jej terenów wynurzyły się ogry i inne, rzadziej spotykane stworzenia. Podjęły one samobójczą, z góry przegraną walkę z nowym uzurpatorem. Z roku na rok organizowane były polowania na Yeti, a sala tronowa Marbusa szybko pokryła się trofeami z ich głów. Kolejna rasa upadła pod ciężkimi butami orków.</t>
+  </si>
+  <si>
+    <t>Gdy Wielka Horda została rozbita, a potęga orków ponownie przeszła do historii, ogry i Yeti wynurzyły się ze swoich pieczar, by walczyć przeciwko elfickim jarlom. Choć zadawały im duże szkody i zabiły wielu wodzów, ich porażka była nieunikniona. Wkrótce łby potworów stały się trofeami na ścianach wielmożów północy, którzy traktowali owe stworzenia wyłącznie jako zwierzynę łowną.</t>
+  </si>
+  <si>
+    <t>Gdy Wielka Horda została rozbita, a potęga orków ponownie przeszła do historii, ogry, Yeti i inne, dzikie rasy północy umknęły w niedostępne dla elfów tereny, gdzie potajemnie mnożyły się bądź wymierały. Wkrótce przeszły do historii, a w kolejnych latach – do legend i bajek dla dzieci. Jarlowie wyparli pamięć o nich, by jeszcze bardziej przyporządkować sobie północne kraje.</t>
   </si>
 </sst>
 </file>
@@ -8832,8 +8835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8867,179 +8870,179 @@
     </row>
     <row r="3" spans="1:3" ht="127.5">
       <c r="B3" s="16" t="s">
-        <v>1211</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="114.75">
       <c r="B4" s="16" t="s">
-        <v>1212</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="102">
       <c r="B5" s="16" t="s">
-        <v>1213</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="102">
       <c r="B6" s="16" t="s">
-        <v>1214</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="114.75">
       <c r="B7" s="16" t="s">
-        <v>1215</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="127.5">
       <c r="B8" s="16" t="s">
-        <v>1216</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="153">
       <c r="B9" s="16" t="s">
-        <v>1217</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="127.5">
       <c r="B10" s="16" t="s">
-        <v>1218</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="127.5">
       <c r="B11" s="16" t="s">
-        <v>1219</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="114.75">
       <c r="B12" s="16" t="s">
-        <v>1220</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="102">
       <c r="B13" s="16" t="s">
-        <v>1221</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165.75">
       <c r="B14" s="16" t="s">
-        <v>1222</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165.75">
       <c r="B15" s="16" t="s">
-        <v>1223</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="204">
       <c r="B16" s="16" t="s">
-        <v>1224</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="204">
       <c r="B17" s="16" t="s">
-        <v>1225</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="102">
       <c r="B18" s="16" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="102">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="114.75">
       <c r="B19" s="16" t="s">
-        <v>1227</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="114.75">
       <c r="B20" s="16" t="s">
-        <v>1228</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="114.75">
       <c r="B21" s="16" t="s">
-        <v>1229</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="114.75">
       <c r="B22" s="16" t="s">
-        <v>1230</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="89.25">
       <c r="B23" s="16" t="s">
-        <v>1231</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="114.75">
       <c r="B24" s="16" t="s">
-        <v>1232</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="114.75">
       <c r="B25" s="16" t="s">
-        <v>1233</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="89.25">
       <c r="B26" s="16" t="s">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="140.25">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="127.5">
       <c r="B27" s="16" t="s">
-        <v>1235</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="89.25">
       <c r="B28" s="16" t="s">
-        <v>1236</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="63.75">
       <c r="B29" s="16" t="s">
-        <v>1237</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="76.5">
       <c r="B30" s="16" t="s">
-        <v>1238</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="114.75">
       <c r="B31" s="16" t="s">
-        <v>1239</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="102">
       <c r="A32" t="s">
-        <v>1240</v>
+        <v>1216</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>1241</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="89.25">
       <c r="A33" t="s">
-        <v>1242</v>
+        <v>1218</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>1243</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="89.25">
       <c r="A34" t="s">
-        <v>1244</v>
+        <v>1219</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>1245</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="89.25">
       <c r="A35" t="s">
-        <v>1246</v>
+        <v>1220</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>1247</v>
+        <v>1473</v>
       </c>
     </row>
   </sheetData>
@@ -9056,8 +9059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9080,533 +9083,533 @@
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="33" t="s">
-        <v>1248</v>
+        <v>1221</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>1249</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="16" t="s">
-        <v>1250</v>
+        <v>1223</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>1251</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" s="16" t="s">
-        <v>1252</v>
+        <v>1225</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>1253</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="B5" s="16" t="s">
-        <v>1254</v>
+        <v>1227</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>1255</v>
+        <v>1228</v>
       </c>
       <c r="D5" t="s">
-        <v>1256</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" s="16" t="s">
-        <v>1257</v>
+        <v>1230</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>1258</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" s="16" t="s">
-        <v>1456</v>
+        <v>1429</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>1278</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5">
       <c r="B8" s="16" t="s">
-        <v>1259</v>
+        <v>1232</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>1260</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="B9" s="16" t="s">
-        <v>1261</v>
+        <v>1234</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>1262</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" s="16" t="s">
-        <v>1263</v>
+        <v>1236</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>1264</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" s="16" t="s">
-        <v>1265</v>
+        <v>1238</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>1266</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" s="16" t="s">
-        <v>1267</v>
+        <v>1240</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>1268</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" s="16" t="s">
-        <v>1269</v>
+        <v>1242</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>1270</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" s="34" t="s">
-        <v>1271</v>
+        <v>1244</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>1277</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="16" t="s">
-        <v>1272</v>
+        <v>1245</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>1276</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" s="16" t="s">
-        <v>1273</v>
+        <v>1246</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>1275</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="25.5">
       <c r="B17" s="16" t="s">
-        <v>1274</v>
+        <v>1247</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>1279</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="16" t="s">
-        <v>1280</v>
+        <v>1253</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>1281</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="16" t="s">
-        <v>1282</v>
+        <v>1255</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>1283</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="16" t="s">
-        <v>1284</v>
+        <v>1257</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>1285</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="25.5">
       <c r="B21" s="16" t="s">
-        <v>1286</v>
+        <v>1259</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>1287</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="16" t="s">
-        <v>1288</v>
+        <v>1261</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>1289</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="16" t="s">
-        <v>1290</v>
+        <v>1263</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>1291</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="16" t="s">
-        <v>1292</v>
+        <v>1265</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>1293</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="25.5">
       <c r="B25" s="16" t="s">
-        <v>1294</v>
+        <v>1267</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>1295</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="32" t="s">
-        <v>1296</v>
+        <v>1269</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>1297</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="16" t="s">
-        <v>1298</v>
+        <v>1271</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>1299</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="16" t="s">
-        <v>1300</v>
+        <v>1273</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>1301</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="25.5">
       <c r="B29" s="16" t="s">
-        <v>1302</v>
+        <v>1275</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>1303</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="25.5">
       <c r="B30" s="16" t="s">
-        <v>1304</v>
+        <v>1277</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>1305</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="31" spans="2:3">
       <c r="B31" s="16" t="s">
-        <v>1306</v>
+        <v>1279</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>1307</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="16" t="s">
-        <v>1308</v>
+        <v>1281</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>1309</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="16" t="s">
-        <v>1310</v>
+        <v>1283</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>1311</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="16" t="s">
-        <v>1312</v>
+        <v>1285</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>1313</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="16" t="s">
-        <v>1314</v>
+        <v>1287</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>1315</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="25.5">
       <c r="B36" s="16" t="s">
-        <v>1316</v>
+        <v>1289</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>1317</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="25.5">
       <c r="B37" s="16" t="s">
-        <v>1318</v>
+        <v>1291</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>1319</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="38" spans="2:3">
       <c r="B38" s="16" t="s">
-        <v>1320</v>
+        <v>1293</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>1321</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="B39" s="16" t="s">
-        <v>1322</v>
+        <v>1295</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>1323</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="40" spans="2:3">
       <c r="B40" s="16" t="s">
-        <v>1324</v>
+        <v>1297</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>1325</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="41" spans="2:3">
       <c r="B41" s="16" t="s">
-        <v>1326</v>
+        <v>1299</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>1327</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="16" t="s">
-        <v>1328</v>
+        <v>1301</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>1329</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="25.5">
       <c r="B43" s="16" t="s">
-        <v>1330</v>
+        <v>1303</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>1331</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="B44" s="16" t="s">
-        <v>1332</v>
+        <v>1305</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>1333</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" s="16" t="s">
-        <v>1334</v>
+        <v>1307</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>1335</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="25.5">
       <c r="B46" s="16" t="s">
-        <v>1336</v>
+        <v>1309</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>1337</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" s="16" t="s">
-        <v>1338</v>
+        <v>1311</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>1339</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="48" spans="2:3">
       <c r="B48" s="16" t="s">
-        <v>1340</v>
+        <v>1313</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>1341</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="49" spans="2:3">
       <c r="B49" s="16" t="s">
-        <v>1342</v>
+        <v>1315</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>1343</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="B50" s="16" t="s">
-        <v>1344</v>
+        <v>1317</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>1345</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="25.5">
       <c r="B51" s="16" t="s">
-        <v>1346</v>
+        <v>1319</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>1347</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="25.5">
       <c r="B52" s="16" t="s">
-        <v>1348</v>
+        <v>1321</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>1349</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" s="16" t="s">
-        <v>1350</v>
+        <v>1323</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>1351</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" s="16" t="s">
-        <v>1352</v>
+        <v>1325</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>1353</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="B55" s="16" t="s">
-        <v>1354</v>
+        <v>1327</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>1355</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="16" t="s">
-        <v>1356</v>
+        <v>1329</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>1357</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="B57" s="16" t="s">
-        <v>1358</v>
+        <v>1331</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>1359</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="25.5">
       <c r="B58" s="16" t="s">
-        <v>1360</v>
+        <v>1333</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>1361</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="B59" s="16" t="s">
-        <v>1362</v>
+        <v>1335</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>1363</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="114.75">
       <c r="B60" s="35" t="s">
-        <v>1457</v>
+        <v>1430</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>1364</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="62" spans="2:3">
       <c r="B62" s="16" t="s">
-        <v>1365</v>
+        <v>1338</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>1366</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="63" spans="2:3">
       <c r="B63" s="16" t="s">
-        <v>1367</v>
+        <v>1340</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>1368</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="64" spans="2:3">
       <c r="B64" s="16" t="s">
-        <v>1370</v>
+        <v>1343</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>1369</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="B65" s="16" t="s">
-        <v>1371</v>
+        <v>1344</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>1372</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="66" spans="2:3">
       <c r="B66" s="16" t="s">
-        <v>1373</v>
+        <v>1346</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>1374</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="B67" s="16" t="s">
-        <v>1375</v>
+        <v>1348</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>1376</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="B68" s="16" t="s">
-        <v>1377</v>
+        <v>1350</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>1378</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="69" spans="2:3">
@@ -9614,15 +9617,15 @@
         <v>4</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>1379</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="B70" s="16" t="s">
-        <v>1380</v>
+        <v>1353</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>1381</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="71" spans="2:3">
@@ -9630,7 +9633,7 @@
         <v>346</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>1382</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="72" spans="2:3">
@@ -9638,127 +9641,132 @@
         <v>488</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>1383</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="73" spans="2:3">
       <c r="B73" s="16" t="s">
-        <v>1384</v>
+        <v>1357</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>1385</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="74" spans="2:3">
       <c r="B74" s="16" t="s">
-        <v>1386</v>
+        <v>1359</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>1387</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="75" spans="2:3">
       <c r="B75" s="16" t="s">
-        <v>1388</v>
+        <v>1361</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>1389</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="76" spans="2:3">
       <c r="B76" s="16" t="s">
-        <v>1390</v>
+        <v>1363</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>1391</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="77" spans="2:3">
       <c r="B77" s="16" t="s">
-        <v>1392</v>
+        <v>1365</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>1393</v>
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80" s="16" t="s">
+        <v>1446</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="16" t="s">
-        <v>1365</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" s="16" t="s">
-        <v>1458</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="83" spans="2:2">
       <c r="B83" s="16" t="s">
-        <v>1459</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="84" spans="2:2">
       <c r="B84" s="16" t="s">
-        <v>1460</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="85" spans="2:2">
       <c r="B85" s="16" t="s">
-        <v>1461</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="86" spans="2:2">
       <c r="B86" s="16" t="s">
-        <v>1462</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" s="16" t="s">
-        <v>1463</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="88" spans="2:2">
       <c r="B88" s="16" t="s">
-        <v>1464</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="89" spans="2:2">
       <c r="B89" s="16" t="s">
-        <v>1465</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="90" spans="2:2">
       <c r="B90" s="16" t="s">
-        <v>1466</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="91" spans="2:2">
       <c r="B91" s="16" t="s">
-        <v>1467</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="92" spans="2:2">
       <c r="B92" s="16" t="s">
-        <v>1468</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="93" spans="2:2">
       <c r="B93" s="16" t="s">
-        <v>1469</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="94" spans="2:2">
       <c r="B94" s="16" t="s">
-        <v>1470</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="95" spans="2:2">
       <c r="B95" s="16" t="s">
-        <v>1471</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="96" spans="2:2">
       <c r="B96" s="16" t="s">
-        <v>1472</v>
+        <v>1445</v>
       </c>
     </row>
   </sheetData>
@@ -14867,7 +14875,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>1407</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="114.75">
@@ -15363,7 +15371,7 @@
         <v>1095</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>1394</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="32.25" customHeight="1">
@@ -15371,7 +15379,7 @@
         <v>1099</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>1395</v>
+        <v>1368</v>
       </c>
       <c r="C63" s="16" t="s">
         <v>1100</v>
@@ -15393,7 +15401,7 @@
         <v>1099</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>1396</v>
+        <v>1369</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>1102</v>
@@ -15404,7 +15412,7 @@
         <v>1103</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>1397</v>
+        <v>1370</v>
       </c>
       <c r="C66" s="16" t="s">
         <v>1104</v>
@@ -15415,7 +15423,7 @@
         <v>1103</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>1398</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="51">
@@ -15423,7 +15431,7 @@
         <v>1103</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>1399</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="38.25">
@@ -15431,7 +15439,7 @@
         <v>1105</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>1400</v>
+        <v>1373</v>
       </c>
       <c r="C69" s="16" t="s">
         <v>1106</v>
@@ -15442,7 +15450,7 @@
         <v>1105</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>1401</v>
+        <v>1374</v>
       </c>
       <c r="C70" s="36" t="s">
         <v>1107</v>
@@ -15482,7 +15490,7 @@
         <v>1112</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>1402</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="38.25">
@@ -15490,7 +15498,7 @@
         <v>1112</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>1403</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="25.5">
@@ -15543,7 +15551,7 @@
         <v>1114</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>1404</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="76.5">
@@ -15551,7 +15559,7 @@
         <v>1114</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>1405</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -15611,7 +15619,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>1406</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="114.75">
@@ -15627,7 +15635,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>1408</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="102">
@@ -15635,7 +15643,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1409</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -15755,7 +15763,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>1410</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="89.25">
@@ -15771,7 +15779,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>1411</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -15790,7 +15798,7 @@
         <v>1136</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>1412</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="102">
@@ -15798,7 +15806,7 @@
         <v>1136</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>1413</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="38.25">
@@ -15806,7 +15814,7 @@
         <v>1136</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>1414</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="76.5">
@@ -15814,7 +15822,7 @@
         <v>1136</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>1415</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -15846,7 +15854,7 @@
         <v>1139</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>1416</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="25.5">
@@ -15873,7 +15881,7 @@
         <v>1142</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>1417</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -15953,7 +15961,7 @@
         <v>1153</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>1418</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="89.25">
@@ -15961,7 +15969,7 @@
         <v>1153</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>1419</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="51">
@@ -15969,7 +15977,7 @@
         <v>1153</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>1420</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="76.5">
@@ -15977,7 +15985,7 @@
         <v>1153</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>1421</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -16009,7 +16017,7 @@
         <v>1153</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>1422</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -16065,7 +16073,7 @@
         <v>1153</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>1423</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -16105,7 +16113,7 @@
         <v>1153</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>1424</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -16113,7 +16121,7 @@
         <v>1153</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>1425</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="89.25">
@@ -16121,7 +16129,7 @@
         <v>1153</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>1426</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="38.25">
@@ -16129,7 +16137,7 @@
         <v>1153</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>1427</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="63.75">
@@ -16161,7 +16169,7 @@
         <v>1170</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>1428</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="38.25">
@@ -16169,7 +16177,7 @@
         <v>1170</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>1429</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="51">
@@ -16177,7 +16185,7 @@
         <v>1170</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>1430</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="89.25">
@@ -16185,7 +16193,7 @@
         <v>1170</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>1431</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="25.5">
@@ -16201,7 +16209,7 @@
         <v>1172</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>1432</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="25.5">
@@ -16209,7 +16217,7 @@
         <v>1172</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>1433</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -16233,7 +16241,7 @@
         <v>1175</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>1434</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="38.25">
@@ -16257,7 +16265,7 @@
         <v>1175</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>1435</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="25.5">
@@ -16265,7 +16273,7 @@
         <v>1175</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>1436</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -16289,7 +16297,7 @@
         <v>1179</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>1437</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="51">
@@ -16297,7 +16305,7 @@
         <v>1179</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>1438</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -16337,7 +16345,7 @@
         <v>1185</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>1439</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -16393,7 +16401,7 @@
         <v>39</v>
       </c>
       <c r="B100" s="37" t="s">
-        <v>1440</v>
+        <v>1413</v>
       </c>
       <c r="D100" t="s">
         <v>1192</v>
@@ -16420,7 +16428,7 @@
         <v>39</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>1441</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="51">
@@ -16428,7 +16436,7 @@
         <v>39</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>1442</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="89.25">
@@ -16468,7 +16476,7 @@
         <v>1198</v>
       </c>
       <c r="B109" s="16" t="s">
-        <v>1443</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="25.5">
@@ -16476,7 +16484,7 @@
         <v>1198</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>1444</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="25.5">
@@ -16492,7 +16500,7 @@
         <v>1201</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>1445</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="51">
@@ -16500,7 +16508,7 @@
         <v>1201</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>1446</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="63.75">
@@ -16508,7 +16516,7 @@
         <v>1202</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>1447</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="63.75">
@@ -16516,7 +16524,7 @@
         <v>1202</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>1448</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="63.75">
@@ -16524,7 +16532,7 @@
         <v>1202</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>1449</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="89.25">
@@ -16532,7 +16540,7 @@
         <v>1202</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>1450</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="63.75">
@@ -16540,7 +16548,7 @@
         <v>1202</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>1451</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="63.75">
@@ -16556,7 +16564,7 @@
         <v>1202</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>1452</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="63.75">
@@ -16564,7 +16572,7 @@
         <v>1202</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>1453</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="25.5">
@@ -16596,7 +16604,7 @@
         <v>1206</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>1454</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -16612,7 +16620,7 @@
         <v>1206</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>1455</v>
+        <v>1428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodanie tłumaczeń scenariusza 11
</commit_message>
<xml_diff>
--- a/storyboard and dialogues/Tłumaczenia Wydry/Reszta polskich poprawek.xlsx
+++ b/storyboard and dialogues/Tłumaczenia Wydry/Reszta polskich poprawek.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frankiewiczp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D29D16-27E7-4041-AA6A-25D1E15CC8AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="10185" tabRatio="500" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27855" windowHeight="12885" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="07" sheetId="1" r:id="rId1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2295" uniqueCount="1597">
   <si>
     <t>Event/Description</t>
   </si>
@@ -7154,11 +7153,380 @@
   <si>
     <t>Gdy Wielka Horda została rozbita, a potęga orków ponownie przeszła do historii, ogry, Yeti i inne, dzikie rasy północy umknęły w niedostępne dla elfów tereny, gdzie potajemnie mnożyły się bądź wymierały. Wkrótce przeszły do historii, a w kolejnych latach – do legend i bajek dla dzieci. Jarlowie wyparli pamięć o nich, by jeszcze bardziej przyporządkować sobie północne kraje.</t>
   </si>
+  <si>
+    <t>Later that day was called ”the Defence of the North” or ”The Battle of Five Armies”. Never before did all the forces of the northern lands unite to fight against a common enemy. And never after.</t>
+  </si>
+  <si>
+    <t>Everyone gave in to the hero mood, and the representatives of all the races danced, sang, ate and drank, boated about their courage and patted each other proudly on their backs. This state of affairs didn’t last for long. The undead threat was still real, and when it became clear that they were hunting for the orcs, numerous elves, humans and dwarves, all wanted them to be gone as soon as possible. If it hadn’t been for Beatrice who was able to restrain the anger of the elven yarls and the noble houses of the Northern Alliance, inarguably there would have been a battle.</t>
+  </si>
+  <si>
+    <t>While no one allowed for open hostility, unfavourable glances and words were harassing the Great Horde all the time. The orcs tolerated them patiently, as they were happy with the warmth of the bonfires, food and the access to medicine. However, Marbus was aware that this would not last forever, and Gewold and the rest of the elders constantly reminded him of that. The key for the Horde was to defeat the King of Gon and to leave.</t>
+  </si>
+  <si>
+    <t>Two weeks after the battle, Marbus and his army were standing in front of the cave entrance where the Gjallarhorn was to be hidden. Not expecting many dangers and not wanting to lead too many troops in the cave, the Great Sovereign assembled his most trusted warriors and set forth into the darkness.</t>
+  </si>
+  <si>
+    <t>And so this is the place where the Gjallarhorn is hidden. Time hasn’t been kind to it: the area is marshy and unstable in many places. This is similar to a elven tample rather than the catacombs I had visited.</t>
+  </si>
+  <si>
+    <t>It should be remembered that this area has been inhabited by the treants for ages. She wouldn’t be surprised if some of these have been hiding here. We should be careful.</t>
+  </si>
+  <si>
+    <t>I sense a beguiling and malicious aura here. We will definitely come across somebody here. Somebody who does not wish us too well. Tread carefully.</t>
+  </si>
+  <si>
+    <t>The elves must have lead uus into a trap! We can’t be sure whether this is the right cave. There must be at least a hundred of archers deep inside.</t>
+  </si>
+  <si>
+    <t>Calm down, Gewold! The elves want to retrieve the horn as much as we do. They wouldn’t turn their backs on us in such a moment. All the yarls have pledged not to be a threat to us.</t>
+  </si>
+  <si>
+    <t>The division into yarls has existed here for not too long. Even though the elves seem to be quite a sensible race, I have lived on this vale of tears much longer and I tell you: you will not find a more quarrelsome family than the elven one. We ought to simply be careful, we might get around without any killing.</t>
+  </si>
+  <si>
+    <t>Cave be wet, much mushroom inside … Mushroom good for the belly, but not good for sleep. That cave be bad for trolls. Trolls likes this more drier … Caverns.</t>
+  </si>
+  <si>
+    <t>She senses a lot of humidity here. She wonders if it’s been like that all the time? Maybe the elves have sunken these lands on purpose in order to get rid of the remains of the orcish culture?</t>
+  </si>
+  <si>
+    <t>Rocks wet, walls wet … Humidity not good for trolls. It getting in the bines and hurting. Knees especially.</t>
+  </si>
+  <si>
+    <t>What the …?!</t>
+  </si>
+  <si>
+    <t>Haha! You have come right into my trap, fools! You even haven’t taken more troops  … Simpletons!</t>
+  </si>
+  <si>
+    <t>Your Yarls promised us safety! You’ve betrayed us! Do you really want to squander your only chance to defeat the undead only to get rid of us?</t>
+  </si>
+  <si>
+    <t>Our Yarls? Our? Ah no … We do not fall under the yarls’ command, neither the witches nor the lords! We are absolutely free!  You stand before the descendant of the Great Landar, the Red Riding Hood (nie pamiętam jak to wcześniej tłumaczyłem?), the ruler of the Blood Elves!</t>
+  </si>
+  <si>
+    <t>The Red Riding Hood? But that a fairy tale for children!</t>
+  </si>
+  <si>
+    <t>Red … Riding Hood … Fairy tale!</t>
+  </si>
+  <si>
+    <t>She used to tell her daughters the story of the Red Riding Hood and the wolf … She didn’t think that there was a grain of truth in it. Where does this nickname come from, elvish girl?</t>
+  </si>
+  <si>
+    <t>One night my former Yarl sent me and my unit to hunt. The fool wanted some deer meat, and we, little dogs, had to rush and hunt some for him. We didn’t expect to be attacked by wolves, or rather your stunted brothers on wolves. Supposedly one of them lead to your wandering our forests now, and we can’t slaughter you like ducks!</t>
+  </si>
+  <si>
+    <t>It doesn’t matter anymore … Coming back to the main story: we weren’t going to surrender without  a fight. We didn’t think of losing at all. And we won, having only our hunting bows and skinnig knives on us. We defeated a pack of wargs, and when we finished … our hoods were red with blood. That thus my nickname.</t>
+  </si>
+  <si>
+    <t>This is a very interesting story, but this jabbering won’t make anyone die, and my sword would gladly taste some of your elvish flesh!</t>
+  </si>
+  <si>
+    <t>This does not have to end like this, girl … You are very young, I will firgive you this excess. Take your warriors and go back home.</t>
+  </si>
+  <si>
+    <t>What! You forgive me!? Our races have fought each other for ages, and I am not going to change this tradition. We will slaughter you! Arrows on the bowstrings!</t>
+  </si>
+  <si>
+    <t>Awww … Bloody hell! Go on, do it! What am I waiting for? Maybe you have no courage to kill an elvish girl, do you?</t>
+  </si>
+  <si>
+    <t>Let’s smash her head, and hang the body at the entrance to the cave! Let the treants know what fighting us means!</t>
+  </si>
+  <si>
+    <t>You fought bravely, girl … but your life belongs to us now. Greath Soveregin?</t>
+  </si>
+  <si>
+    <t>It think that …</t>
+  </si>
+  <si>
+    <t>we should kill the girl and teach the elves a lesson!</t>
+  </si>
+  <si>
+    <t>we should set her free as a sign of good will!</t>
+  </si>
+  <si>
+    <t>Butcher her. And do so with the rest of this elvish litter! Let’s spill the elvish blood!</t>
+  </si>
+  <si>
+    <t>My death won’t change anything! Be cursed, Marbus! I swear I will haunt you even from the grave!</t>
+  </si>
+  <si>
+    <t>Ha ha! Problem solved!</t>
+  </si>
+  <si>
+    <t>Let the kid go! Let her go back to her people. Perhaps when her anger subsides and she thinks through her behaviour , she will understand her foolish actions … We can’t kill everyone who isn’t favourable towards us. The undead are our enemy, not the elves!</t>
+  </si>
+  <si>
+    <t>Ha! You think this will change anything? I will hunt you until the end of my days and will never let you have any rest! I swear I will kill every orc I come across!</t>
+  </si>
+  <si>
+    <t>Foolishness! If  I were in command of the Great Horde, such an excess wouldn’t happen! This only shows that even elvish pups can oppose us without any consequences!</t>
+  </si>
+  <si>
+    <t>But you are not in command of the Great Horde, Gewold … And you’d better remember about it.</t>
+  </si>
+  <si>
+    <t>Treants! Humidity, muchroom, elves … Kill all bad elves and escape as fast as we can!</t>
+  </si>
+  <si>
+    <t>And so more enemy forces? When will these fools understand that all races should unite against the common enemy?</t>
+  </si>
+  <si>
+    <t>She prepares for a fight …</t>
+  </si>
+  <si>
+    <t>More elves? Great, simply fabulous! Come to me, my friends! Daddy has somethign for you … A big blade which will gut each of you!</t>
+  </si>
+  <si>
+    <t>The south room … Darn, even here, too? Everyone, to me, we need to clear this area! I’m almost sure that we will find something here!</t>
+  </si>
+  <si>
+    <t>Humidity! It comes from here! A lakey! And this means fishes! Trolls likes fishes! There is fishes, fish-woman?</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>She is not … But yes, there is fish here. Collurful. She saw such fish a long time ago, near the coral reefs.</t>
+  </si>
+  <si>
+    <t>Ree … What?</t>
+  </si>
+  <si>
+    <t>These are … like gardens .. under water, under vast, salty water. She thinks this pool is magical, heals wounds … It reminds the body what is should be: healed.</t>
+  </si>
+  <si>
+    <t>Great! We can use this place to heal. It seems to me we won’t find anything better here.</t>
+  </si>
+  <si>
+    <t>This spring is not natural. Someone created it here. Someone opened the ground and ordered it to gush out magical healing water. I myself cannot tell whether it’s been done by an elvish mage or an orcish shaman.</t>
+  </si>
+  <si>
+    <t>I’d like to believe the second option is true … I have never suspected that my people have such a colourful history. Might orcish fortresses, the curse of the Wild Gon, the Gjallarhorn … I would have never suspected to come across such things … To lead the Great Horde.</t>
+  </si>
+  <si>
+    <t>Sometimes life plays tricks on us, Marbus. We must learn to accept the changes, whatever they are, and then live according to new rules. This pond is the new rule … It only depends on you how you will use it.</t>
+  </si>
+  <si>
+    <t>You are right. Created by orcs or not … It will serve to hea our warriors.</t>
+  </si>
+  <si>
+    <t>She senses a strange aura around the pond. It seems to be healing wounds.</t>
+  </si>
+  <si>
+    <t>Excellent! It will make do for our wounded warriors. Keep it safe.</t>
+  </si>
+  <si>
+    <t>This is a glyph … We’d better take it with us. I bet we will become useful.</t>
+  </si>
+  <si>
+    <t>What the …? A stone? Some magical contraption … I may be useful.</t>
+  </si>
+  <si>
+    <t>She has found the glyph. I will no doubt be useful for finding the Gjallarhorn.</t>
+  </si>
+  <si>
+    <t>A magical stone … I feel we will find it useful.</t>
+  </si>
+  <si>
+    <t>What the…?!</t>
+  </si>
+  <si>
+    <t>Waaaargh! Leave my cave be! What do you want from it?</t>
+  </si>
+  <si>
+    <t>We are looking for the Gjallarhorn. We are not going to stay her for long.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeah, sure! First, the elves came and mollified me with their elvish food, but they won’t leave! You’ve left their corpses, and the soil has already soaked up the blood. You will pay for devastating my dwelling! </t>
+  </si>
+  <si>
+    <t>Draw your swords!</t>
+  </si>
+  <si>
+    <t>Cursed orcs! Wherever you turn up … death always follows!</t>
+  </si>
+  <si>
+    <t>He is truly right. But it’s time to ease ourselves of this curse’s burden. Let’s take the glyph and try using it somehow.</t>
+  </si>
+  <si>
+    <t>This statue looks different from the rest. There seems to be a passage behind it. Meybe we could move it aside …</t>
+  </si>
+  <si>
+    <t>What for? Let’s call some hefty-looking soldiers and take a batternig ram. It will yield.</t>
+  </si>
+  <si>
+    <t>This is not the best idea. When I was in the catacombs of the stronghold, I came across some scriptures telling about such passages. If we use force to move the statue, the cave will collapse and finding the Gjallarhorn will take us months. Assuming, of course, it is still there.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What shall we do, then? Call the elvish witch so that she will cast a spell and unblock the passage for us? </t>
+  </si>
+  <si>
+    <t>She thinks it won’t be necessary. Look at the statue: it seems to be possible to be filled with something… A crystal of sorts …. or glyphs. We might find them here and they will open the passage.</t>
+  </si>
+  <si>
+    <t>Aidala is right. Let’s have a look around the cave and come back here when we find something.</t>
+  </si>
+  <si>
+    <t>This statue looks different from the rest. There seems to be a passage behind it. Maybe we could move it aside …</t>
+  </si>
+  <si>
+    <t>She thinks it won’t be necessary. Look at the statue: it seems to be possible to be filled with something… A crystal of sorts …. or glyphs. Why don’t we put the stones we found in the spaces on the statue. However, we will have to do it in the right order.</t>
+  </si>
+  <si>
+    <t>Over the spaces there are some words carved. This can be a riddle.</t>
+  </si>
+  <si>
+    <t>The biggest sign</t>
+  </si>
+  <si>
+    <t>Damn it, not this way. Let’s start over.</t>
+  </si>
+  <si>
+    <t>Enter the glyph with the letter L</t>
+  </si>
+  <si>
+    <t>Enter the glyph with the letter C</t>
+  </si>
+  <si>
+    <t>Enter the glyph with the letter U</t>
+  </si>
+  <si>
+    <t>Enter the glyph with the letter S</t>
+  </si>
+  <si>
+    <t>Enter the glyph with the letter B</t>
+  </si>
+  <si>
+    <t>We’ve made it! The statue is moving!</t>
+  </si>
+  <si>
+    <t>She is thinking of a password … CLUBS … Oh yes, it we look at the shape of the cave…</t>
+  </si>
+  <si>
+    <t>This is of no importance! Let’s take the horn and set out to deal with the Wild Gon!</t>
+  </si>
+  <si>
+    <t>I’m afraid this is not the end of the dangers … But it’s true, it’s time to set off. Follow me!</t>
+  </si>
+  <si>
+    <t>Finally, we’ve collected all the glyphs. It’s time to have a look at the statue.</t>
+  </si>
+  <si>
+    <t>A rat! Dinner!</t>
+  </si>
+  <si>
+    <t>Filthy rodent! Some you fry them over fire and eat, but I’ve never manager to look a it! Disgusting!</t>
+  </si>
+  <si>
+    <t>She has a question …</t>
+  </si>
+  <si>
+    <t>Yes, Aidala?</t>
+  </si>
+  <si>
+    <t>Can we keep it?</t>
+  </si>
+  <si>
+    <t>What ?!</t>
+  </si>
+  <si>
+    <t>The rat. Can we keep it? It is so sweet and … shaggy.</t>
+  </si>
+  <si>
+    <t>Ehh… This doesn’t seem to be a good idea. It can have rabies and pass it on to our army. But I can bring you an animal when all of this ends.</t>
+  </si>
+  <si>
+    <t>Very well, Marbus.</t>
+  </si>
+  <si>
+    <t>Barley is shaggy, too. However, it’s hard to call him sweet …</t>
+  </si>
+  <si>
+    <t>… or it isn’t.</t>
+  </si>
+  <si>
+    <t>But it’s your animal. I want one of my own.</t>
+  </si>
+  <si>
+    <t>Cursed flying rats! I can never shoot them! Waaargh!</t>
+  </si>
+  <si>
+    <t>She thinks you should be using some sedatives.</t>
+  </si>
+  <si>
+    <t>She thinks it’s high time to be ready for a hard battle …</t>
+  </si>
+  <si>
+    <t>Maybe not … He is probably …. Sleeping?</t>
+  </si>
+  <si>
+    <t>Sharpen your swords! Now we have the chance! Uproot the treant!</t>
+  </si>
+  <si>
+    <t>What … what …? What!? Who dares enter Clubs’s dwelling!?</t>
+  </si>
+  <si>
+    <t>And all our plan fell apart… I’m Marbus, The Great Sovereign of the Horde. I’ve come here to take the Gjallarhorn thanks to which we can destroy the King of Wild Gon and lift the curse from my race.</t>
+  </si>
+  <si>
+    <t>It’s fine … If you are telling the truth, I have been sleeping here for thousand years. I bacace the guardian of this place and was planted but an orc shaman, one of your predecessors. He must have gathered the Great Horde and deafeated the King of Gon. What he did then was, however, very imprudent.</t>
+  </si>
+  <si>
+    <t>Imprudent? What do you mean, guardian?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The orc thought that he would be able to break the curse of the Wild Gond once and for all. He lived long. Very long. He was a great mage. He understood the true nature of the Curse. It draw its strength from the orcush nature itself, your wickedness and bloodthirst. It was supposed to be the final weapon against your kind, which was made by the beings across the ocean. </t>
+  </si>
+  <si>
+    <t>But the orc created a magical object, thanks to which the curse could be lifted for one thousand years. And yes, the object is the Gjallarhorn. After many years, the mage came to the conclusion that this was not enough. He created an amulet allowing you to bind the curse to you, take its burden upon oneself. The burden of the sins of the orcish race …</t>
+  </si>
+  <si>
+    <t>Such a great sacrifice … What happened next?</t>
+  </si>
+  <si>
+    <t>The shaman made ghis amulet at the dwarfish smithies, using the best tools the dwarves had. He worked hard for many months, and his warriors withstood the dwarfish siege. In the end they lost, and the mage fled. He was killed by the beardmen in a forgotten tunnel, where his ghost haunts, and the amulet awaits to be found. At least that is what the legend says.</t>
+  </si>
+  <si>
+    <t>So, enough talk. We’ve come for the artifact, so a trial awaits. To battle!</t>
+  </si>
+  <si>
+    <t>Phew … It wasn’t easy. We can finally take the horn and leave.</t>
+  </si>
+  <si>
+    <t>Oh … Such treants are a mere trifle for me. But killing them does not bring any joy. I prefer enemies which are bleeding!</t>
+  </si>
+  <si>
+    <t>You think it is so easy? Before you the the Gjallarhorn, first you have to defeat me!</t>
+  </si>
+  <si>
+    <t>At last! We have it. It’s time to leave the cave. We won’t find anything interesting here, and the Wild Gon is growing in strength with every minute!</t>
+  </si>
+  <si>
+    <t>You thought that would be so easy to do? Oh no, first you have to deal with me!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skeletons dancing in a circle and large stone gates through which warriors with big swords and fangs come out have been carved on the statue. In the background, you there are figures in helmets and full armour who are panicking. </t>
+  </si>
+  <si>
+    <t>Someone carved a battle scene here: figures in full armour are fighting the ones with big swords and fangs… The former are losign sand retreating towards the boat.</t>
+  </si>
+  <si>
+    <t>The scene shows skeleton destroying cities and killing the countrymen, In the background there are orcs building ships and setting out in the sea.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Someone carved twevle skeleton in long robes, all of them with their hands up to the sky, and above them there is something that looks like an eclipse. In the middle of the skeleton circle, a shape of a ghost or a demons is looming. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The low relief shows an orc, but not a typical one. He is holding a staff and a medallion. He is a bit shorter than most orcs, and seems to have a decent amount of goblin blood flowing in his veins. His face is worried, although there is determination in his eyes. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14">
     <font>
       <sz val="10"/>
@@ -7257,7 +7625,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7300,6 +7668,12 @@
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -7314,7 +7688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7424,6 +7798,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7773,7 +8150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK94"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
@@ -8832,10 +9209,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -9056,7 +9433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
@@ -9776,7 +10153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
@@ -10565,7 +10942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
@@ -11407,7 +11784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12439,10 +12816,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D144"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -12481,13 +12860,19 @@
       <c r="B3" s="16" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="127.5">
+      <c r="C3" s="16" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="140.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>664</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>1475</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="102">
@@ -12497,6 +12882,9 @@
       <c r="B5" s="16" t="s">
         <v>665</v>
       </c>
+      <c r="C5" s="16" t="s">
+        <v>1476</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="76.5">
       <c r="A6" t="s">
@@ -12505,6 +12893,9 @@
       <c r="B6" s="16" t="s">
         <v>666</v>
       </c>
+      <c r="C6" s="16" t="s">
+        <v>1477</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -12513,6 +12904,7 @@
       <c r="B7" s="16" t="s">
         <v>667</v>
       </c>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
@@ -12521,6 +12913,7 @@
       <c r="B8" s="16" t="s">
         <v>668</v>
       </c>
+      <c r="C8" s="40"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
@@ -12529,6 +12922,7 @@
       <c r="B9" s="16" t="s">
         <v>669</v>
       </c>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
@@ -12537,6 +12931,7 @@
       <c r="B10" s="16" t="s">
         <v>670</v>
       </c>
+      <c r="C10" s="40"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -12545,6 +12940,7 @@
       <c r="B11" s="16" t="s">
         <v>671</v>
       </c>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
@@ -12553,6 +12949,7 @@
       <c r="B12" s="16" t="s">
         <v>672</v>
       </c>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:3" ht="63.75">
       <c r="A13" t="s">
@@ -12561,6 +12958,9 @@
       <c r="B13" s="16" t="s">
         <v>673</v>
       </c>
+      <c r="C13" s="16" t="s">
+        <v>1478</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="51">
       <c r="A14" t="s">
@@ -12569,6 +12969,9 @@
       <c r="B14" s="16" t="s">
         <v>674</v>
       </c>
+      <c r="C14" s="16" t="s">
+        <v>1479</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
@@ -12577,6 +12980,7 @@
       <c r="B15" s="16" t="s">
         <v>675</v>
       </c>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:3" ht="38.25">
       <c r="A16" t="s">
@@ -12585,6 +12989,9 @@
       <c r="B16" s="16" t="s">
         <v>676</v>
       </c>
+      <c r="C16" s="16" t="s">
+        <v>1480</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="38.25">
       <c r="A17" t="s">
@@ -12593,6 +13000,9 @@
       <c r="B17" s="16" t="s">
         <v>677</v>
       </c>
+      <c r="C17" s="16" t="s">
+        <v>1481</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="51">
       <c r="A18" t="s">
@@ -12601,13 +13011,19 @@
       <c r="B18" s="16" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="63.75">
+      <c r="C18" s="16" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="76.5">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>679</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>1483</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="38.25">
@@ -12617,13 +13033,19 @@
       <c r="B20" s="16" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="38.25">
+      <c r="C20" s="16" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="51">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>681</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>1485</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="25.5">
@@ -12633,6 +13055,9 @@
       <c r="B22" s="16" t="s">
         <v>682</v>
       </c>
+      <c r="C22" s="16" t="s">
+        <v>1486</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
@@ -12657,6 +13082,9 @@
       <c r="B25" s="16" t="s">
         <v>686</v>
       </c>
+      <c r="C25" s="16" t="s">
+        <v>1487</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="25.5">
       <c r="A26" t="s">
@@ -12665,6 +13093,9 @@
       <c r="B26" s="16" t="s">
         <v>687</v>
       </c>
+      <c r="C26" s="16" t="s">
+        <v>1488</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="38.25">
       <c r="A27" t="s">
@@ -12673,13 +13104,19 @@
       <c r="B27" s="16" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="51">
+      <c r="C27" s="16" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="63.75">
       <c r="A28" t="s">
         <v>229</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>689</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>1490</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -12689,6 +13126,9 @@
       <c r="B29" s="16" t="s">
         <v>690</v>
       </c>
+      <c r="C29" s="16" t="s">
+        <v>1491</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
@@ -12697,6 +13137,9 @@
       <c r="B30" s="16" t="s">
         <v>691</v>
       </c>
+      <c r="C30" s="16" t="s">
+        <v>1492</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="51">
       <c r="A31" t="s">
@@ -12705,6 +13148,9 @@
       <c r="B31" s="16" t="s">
         <v>692</v>
       </c>
+      <c r="C31" s="16" t="s">
+        <v>1493</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="102">
       <c r="A32" t="s">
@@ -12713,663 +13159,988 @@
       <c r="B32" s="16" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="89.25">
+      <c r="C32" s="16" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="89.25">
       <c r="A33" t="s">
         <v>229</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="38.25">
+      <c r="C33" s="16" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="38.25">
       <c r="A34" t="s">
         <v>229</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="38.25">
+      <c r="C34" s="16" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="38.25">
       <c r="A35" t="s">
         <v>229</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="38.25">
+      <c r="C35" s="16" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="38.25">
       <c r="A36" t="s">
         <v>229</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="25.5">
+      <c r="C36" s="16" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="25.5">
       <c r="A37" t="s">
         <v>698</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="38.25">
+      <c r="C37" s="16" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="38.25">
       <c r="A38" t="s">
         <v>698</v>
       </c>
       <c r="B38" s="16" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="25.5">
+      <c r="C38" s="16" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="25.5">
       <c r="A39" t="s">
         <v>698</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" s="16" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>698</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" s="16" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>698</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="25.5">
+      <c r="C41" s="16" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="25.5">
       <c r="A42" t="s">
         <v>698</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="38.25">
+      <c r="C42" s="16" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="38.25">
       <c r="A43" t="s">
         <v>698</v>
       </c>
       <c r="B43" s="16" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" s="16" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>698</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" s="16" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>698</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="63.75">
+      <c r="C45" s="16" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="63.75">
       <c r="A46" t="s">
         <v>698</v>
       </c>
       <c r="B46" s="16" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="38.25">
+      <c r="C46" s="16" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="38.25">
       <c r="A47" t="s">
         <v>698</v>
       </c>
       <c r="B47" s="16" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="51">
+      <c r="C47" s="16" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="51">
       <c r="A48" t="s">
         <v>698</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="25.5">
+      <c r="C48" s="16" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="25.5">
       <c r="A49" t="s">
         <v>698</v>
       </c>
       <c r="B49" s="16" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="25.5">
+      <c r="C49" s="16" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="25.5">
       <c r="A50" t="s">
         <v>698</v>
       </c>
       <c r="B50" s="16" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="38.25">
+      <c r="C50" s="16" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="38.25">
       <c r="A51" t="s">
         <v>698</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" s="16" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>698</v>
       </c>
       <c r="B52" s="16" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="38.25">
+      <c r="C52" s="16" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="38.25">
       <c r="A53" t="s">
         <v>229</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="38.25">
+      <c r="C53" s="16" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="38.25">
       <c r="A54" t="s">
         <v>229</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="25.5">
+      <c r="C54" s="16" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="25.5">
       <c r="B55" s="16" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" s="16" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="B56" s="16" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="38.25">
+      <c r="C56" s="16" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="38.25">
       <c r="B57" s="16" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" s="16" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="B58" s="16" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="38.25">
+      <c r="C58" s="16" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="38.25">
       <c r="B59" s="16" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="38.25">
+      <c r="C59" s="16" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="25.5">
       <c r="B60" s="16" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="25.5">
+        <v>722</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="51">
       <c r="B61" s="16" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="51">
+        <v>723</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="63.75">
       <c r="B62" s="16" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="63.75">
+        <v>724</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="51">
       <c r="B63" s="16" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="51">
+        <v>725</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="25.5">
       <c r="B64" s="16" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="25.5">
+        <v>726</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="25.5">
       <c r="B65" s="16" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="25.5">
+        <v>727</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="25.5">
       <c r="B66" s="16" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="25.5">
+        <v>728</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="B67" s="16" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>729</v>
+      </c>
+      <c r="C67" s="40"/>
+    </row>
+    <row r="68" spans="1:3" ht="25.5">
       <c r="B68" s="16" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="25.5">
+        <v>730</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="25.5">
       <c r="B69" s="16" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="25.5">
+        <v>731</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="25.5">
       <c r="B70" s="16" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="25.5">
+        <v>732</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="B71" s="16" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>733</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="B72" s="16" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>734</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="B73" s="16" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>686</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="B74" s="16" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>735</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="25.5">
       <c r="B75" s="16" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="25.5">
+        <v>736</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="51">
       <c r="B76" s="16" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="51">
+        <v>737</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="B77" s="16" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>738</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="25.5">
+      <c r="A78" t="s">
+        <v>739</v>
+      </c>
       <c r="B78" s="16" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="25.5">
+        <v>740</v>
+      </c>
+      <c r="C78" s="16" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="38.25">
       <c r="A79" t="s">
         <v>739</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="25.5">
+        <v>741</v>
+      </c>
+      <c r="C79" s="16" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="25.5">
       <c r="A80" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="25.5">
+        <v>743</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="25.5">
       <c r="A81" t="s">
         <v>742</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="25.5">
+        <v>744</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="76.5">
       <c r="A82" t="s">
         <v>742</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="76.5">
+        <v>745</v>
+      </c>
+      <c r="C82" s="16" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="25.5">
       <c r="A83" t="s">
         <v>742</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="25.5">
+        <v>746</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="51">
       <c r="A84" t="s">
         <v>742</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="51">
+        <v>747</v>
+      </c>
+      <c r="C84" s="16" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="25.5">
       <c r="A85" t="s">
         <v>742</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="25.5">
+        <v>748</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="25.5">
       <c r="A86" t="s">
-        <v>742</v>
+        <v>749</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="25.5">
-      <c r="A87" t="s">
-        <v>749</v>
-      </c>
+        <v>750</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="25.5">
       <c r="B87" s="16" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="25.5">
+        <v>751</v>
+      </c>
+      <c r="C87" s="16" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="25.5">
       <c r="B88" s="16" t="s">
+        <v>752</v>
+      </c>
+      <c r="C88" s="16" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="25.5">
+      <c r="B89" s="16" t="s">
+        <v>744</v>
+      </c>
+      <c r="C89" s="16" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="76.5">
+      <c r="B90" s="16" t="s">
+        <v>745</v>
+      </c>
+      <c r="C90" s="16" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="25.5">
+      <c r="B91" s="16" t="s">
+        <v>746</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="63.75">
+      <c r="B92" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="C92" s="16" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="25.5">
+      <c r="B93" s="16" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" ht="25.5">
-      <c r="B89" s="16" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="25.5">
-      <c r="B90" s="16" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="76.5">
-      <c r="B91" s="16" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="25.5">
-      <c r="B92" s="16" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="63.75">
-      <c r="B93" s="16" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="25.5">
+      <c r="C93" s="16" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="B94" s="16" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>754</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="B95" s="16" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>755</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="B96" s="16" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2">
+        <v>756</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3">
       <c r="B97" s="16" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2">
+        <v>757</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3">
       <c r="B98" s="16" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2">
+        <v>758</v>
+      </c>
+      <c r="C98" s="16" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3">
       <c r="B99" s="16" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2">
+        <v>759</v>
+      </c>
+      <c r="C99" s="16" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3">
       <c r="B100" s="16" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2">
+        <v>760</v>
+      </c>
+      <c r="C100" s="16" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3">
       <c r="B101" s="16" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2">
+        <v>761</v>
+      </c>
+      <c r="C101" s="16" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" ht="25.5">
       <c r="B102" s="16" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" ht="25.5">
+        <v>762</v>
+      </c>
+      <c r="C102" s="16" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" ht="25.5">
       <c r="B103" s="16" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" ht="25.5">
+        <v>763</v>
+      </c>
+      <c r="C103" s="16" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" ht="25.5">
       <c r="B104" s="16" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" ht="25.5">
+        <v>764</v>
+      </c>
+      <c r="C104" s="16" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3">
       <c r="B105" s="16" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2">
+        <v>765</v>
+      </c>
+      <c r="C105" s="16" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" ht="38.25">
       <c r="B106" s="16" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" ht="38.25">
+        <v>766</v>
+      </c>
+      <c r="C106" s="16" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3">
       <c r="B107" s="16" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2">
+        <v>767</v>
+      </c>
+      <c r="C107" s="16" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3">
       <c r="B108" s="16" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2">
+        <v>768</v>
+      </c>
+      <c r="C108" s="16" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3">
       <c r="B109" s="16" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2">
+        <v>769</v>
+      </c>
+      <c r="C109" s="16" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3">
       <c r="B110" s="16" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2">
+        <v>770</v>
+      </c>
+      <c r="C110" s="16" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" ht="25.5">
       <c r="B111" s="16" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="112" spans="2:2" ht="25.5">
+        <v>771</v>
+      </c>
+      <c r="C111" s="16" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" ht="25.5">
       <c r="B112" s="16" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" ht="25.5">
+        <v>772</v>
+      </c>
+      <c r="C112" s="16" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
       <c r="B113" s="16" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2">
+        <v>773</v>
+      </c>
+      <c r="C113" s="40"/>
+    </row>
+    <row r="114" spans="2:3">
       <c r="B114" s="16" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2">
+        <v>774</v>
+      </c>
+      <c r="C114" s="16" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3">
       <c r="B115" s="16" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2">
+        <v>775</v>
+      </c>
+      <c r="C115" s="16" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" ht="51">
       <c r="B116" s="16" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2" ht="51">
+        <v>776</v>
+      </c>
+      <c r="C116" s="16" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3">
       <c r="B117" s="16" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2">
+        <v>777</v>
+      </c>
+      <c r="C117" s="16" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="25.5">
       <c r="B118" s="16" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" ht="25.5">
+        <v>778</v>
+      </c>
+      <c r="C118" s="16" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3">
       <c r="B119" s="16" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2">
+        <v>779</v>
+      </c>
+      <c r="C119" s="40"/>
+    </row>
+    <row r="120" spans="2:3" ht="25.5">
       <c r="B120" s="16" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" ht="25.5">
+        <v>780</v>
+      </c>
+      <c r="C120" s="16" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" ht="25.5">
       <c r="B121" s="16" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" ht="25.5">
+        <v>781</v>
+      </c>
+      <c r="C121" s="16" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3">
       <c r="B122" s="16" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2">
+        <v>782</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3">
       <c r="B123" s="16" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2">
+        <v>783</v>
+      </c>
+      <c r="C123" s="16" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" ht="25.5">
       <c r="B124" s="16" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2" ht="25.5">
+        <v>784</v>
+      </c>
+      <c r="C124" s="16" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" ht="25.5">
       <c r="B125" s="16" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2" ht="25.5">
+        <v>785</v>
+      </c>
+      <c r="C125" s="16" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" ht="51">
       <c r="B126" s="16" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="127" spans="2:2" ht="51">
+        <v>786</v>
+      </c>
+      <c r="C126" s="16" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" ht="76.5">
       <c r="B127" s="16" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2" ht="63.75">
+        <v>787</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3">
       <c r="B128" s="16" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2">
+        <v>788</v>
+      </c>
+      <c r="C128" s="16" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" ht="63.75" customHeight="1">
       <c r="B129" s="16" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2" ht="63.75" customHeight="1">
+        <v>789</v>
+      </c>
+      <c r="C129" s="16" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" ht="89.25">
       <c r="B130" s="16" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" ht="89.25">
+        <v>790</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3">
       <c r="B131" s="16" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2">
+        <v>791</v>
+      </c>
+      <c r="C131" s="16" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" ht="114.75">
       <c r="B132" s="16" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" ht="81" customHeight="1">
+        <v>792</v>
+      </c>
+      <c r="C132" s="16" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" ht="25.5">
       <c r="B133" s="16" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" ht="25.5">
+        <v>793</v>
+      </c>
+      <c r="C133" s="16" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" ht="25.5">
       <c r="B134" s="16" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" ht="25.5">
+        <v>794</v>
+      </c>
+      <c r="C134" s="16" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" ht="38.25">
       <c r="B135" s="16" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" ht="38.25">
+        <v>795</v>
+      </c>
+      <c r="C135" s="16" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" ht="25.5">
       <c r="B136" s="16" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" ht="25.5">
+        <v>796</v>
+      </c>
+      <c r="C136" s="16" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" ht="38.25">
       <c r="B137" s="16" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2" ht="38.25">
+        <v>797</v>
+      </c>
+      <c r="C137" s="16" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" ht="25.5">
       <c r="B138" s="16" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2" ht="25.5">
+        <v>798</v>
+      </c>
+      <c r="C138" s="16" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" ht="63.75">
       <c r="B139" s="16" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" ht="51">
+        <v>799</v>
+      </c>
+      <c r="C139" s="16" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" ht="38.25">
       <c r="B140" s="16" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" ht="38.25">
+        <v>800</v>
+      </c>
+      <c r="C140" s="16" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" ht="38.25">
       <c r="B141" s="16" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2" ht="38.25">
+        <v>801</v>
+      </c>
+      <c r="C141" s="16" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" ht="63.75">
       <c r="B142" s="16" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2" ht="51">
+        <v>802</v>
+      </c>
+      <c r="C142" s="16" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" ht="63.75">
       <c r="B143" s="16" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2" ht="63.75">
-      <c r="B144" s="16" t="s">
         <v>803</v>
+      </c>
+      <c r="C143" s="16" t="s">
+        <v>1596</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Page &amp;P</oddFooter>
@@ -13378,7 +14149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
@@ -14007,7 +14778,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
@@ -14837,7 +15608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -15581,7 +16352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D127"/>
   <sheetViews>
     <sheetView topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>